<commit_message>
fix: Implemented service & view for schedule
</commit_message>
<xml_diff>
--- a/horario_semestre.xlsx
+++ b/horario_semestre.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Lunes</t>
   </si>
@@ -39,14 +39,14 @@
 Reloj 102</t>
   </si>
   <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>Algoritmos y Complejidad (3)
+Humanidades 202</t>
+  </si>
+  <si>
     <t>Computación Cuántica (A)
-Humanidades 202</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>Algoritmos y Complejidad (3)
 Humanidades 202</t>
   </si>
   <si>
@@ -537,24 +537,22 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -567,10 +565,10 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -583,10 +581,10 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -717,7 +715,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -734,7 +732,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
feat: Alert message when scheduler fail
</commit_message>
<xml_diff>
--- a/horario_semestre.xlsx
+++ b/horario_semestre.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Lunes</t>
   </si>
@@ -33,6 +33,10 @@
   </si>
   <si>
     <t>9:00</t>
+  </si>
+  <si>
+    <t>Diseño de Software Verificable (B2)
+Reloj 102</t>
   </si>
   <si>
     <t>Introducción a la Programación (1)
@@ -42,33 +46,29 @@
     <t>10:00</t>
   </si>
   <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>Introducción a la Programación (2)
+Reloj 103</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>ALMUERZO</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
     <t>Algoritmos y Complejidad (3)
-Humanidades 202</t>
-  </si>
-  <si>
-    <t>Computación Cuántica (A)
-Humanidades 202</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>Introducción a la Programación (2)
-Reloj 102
-Diseño de Software Verificable (B2)
-Reloj 104</t>
-  </si>
-  <si>
-    <t>12:00</t>
-  </si>
-  <si>
-    <t>13:00</t>
-  </si>
-  <si>
-    <t>ALMUERZO</t>
-  </si>
-  <si>
-    <t>14:00</t>
+Reloj 104
+Computación Cuántica (A)
+Ciencias 505</t>
   </si>
   <si>
     <t>15:00</t>
@@ -113,10 +113,13 @@
     <t>Reloj 102</t>
   </si>
   <si>
-    <t>Humanidades 202</t>
+    <t>Reloj 103</t>
   </si>
   <si>
     <t>Reloj 104</t>
+  </si>
+  <si>
+    <t>Ciencias 505</t>
   </si>
 </sst>
 </file>
@@ -535,65 +538,55 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -602,9 +595,11 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -614,7 +609,9 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -624,7 +621,9 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -678,13 +677,13 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -698,13 +697,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -712,16 +711,16 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -729,16 +728,16 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -749,13 +748,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: required fields on modal forms
</commit_message>
<xml_diff>
--- a/horario_semestre.xlsx
+++ b/horario_semestre.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Lunes</t>
   </si>
@@ -36,7 +36,9 @@
   </si>
   <si>
     <t>Introducción a la Programación (1)
-Reloj 102</t>
+Reloj 102
+Introducción a la Programación (2)
+Reloj 103</t>
   </si>
   <si>
     <t>10:00</t>
@@ -45,10 +47,6 @@
     <t>11:00</t>
   </si>
   <si>
-    <t>Introducción a la Programación (2)
-Reloj 102</t>
-  </si>
-  <si>
     <t>12:00</t>
   </si>
   <si>
@@ -62,12 +60,16 @@
   </si>
   <si>
     <t>Algoritmos y Complejidad (3)
+Reloj 103</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>Introducción a la Programación (asdf)
 Ciencias 507</t>
   </si>
   <si>
-    <t>15:00</t>
-  </si>
-  <si>
     <t>16:00</t>
   </si>
   <si>
@@ -98,7 +100,13 @@
     <t>Algoritmos y Complejidad (Sección 3)</t>
   </si>
   <si>
+    <t>Introducción a la Programación (Sección asdf)</t>
+  </si>
+  <si>
     <t>Reloj 102</t>
+  </si>
+  <si>
+    <t>Reloj 103</t>
   </si>
   <si>
     <t>Ciencias 507</t>
@@ -541,9 +549,7 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -551,11 +557,9 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -563,10 +567,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -575,38 +579,42 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -629,7 +637,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -666,7 +674,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -677,13 +685,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -691,16 +699,33 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix de metodos en correccion y proteccon en json
</commit_message>
<xml_diff>
--- a/horario_semestre.xlsx
+++ b/horario_semestre.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Lunes</t>
   </si>
@@ -36,9 +36,7 @@
   </si>
   <si>
     <t>Introducción a la Programación (1)
-Reloj 102
-Introducción a la Programación (2)
-Reloj 103</t>
+Reloj 102</t>
   </si>
   <si>
     <t>10:00</t>
@@ -47,6 +45,10 @@
     <t>11:00</t>
   </si>
   <si>
+    <t>Introducción a la Programación (2)
+Reloj 102</t>
+  </si>
+  <si>
     <t>12:00</t>
   </si>
   <si>
@@ -60,16 +62,12 @@
   </si>
   <si>
     <t>Algoritmos y Complejidad (3)
-Reloj 103</t>
+Ciencias 507</t>
   </si>
   <si>
     <t>15:00</t>
   </si>
   <si>
-    <t>Introducción a la Programación (asdf)
-Ciencias 507</t>
-  </si>
-  <si>
     <t>16:00</t>
   </si>
   <si>
@@ -100,13 +98,7 @@
     <t>Algoritmos y Complejidad (Sección 3)</t>
   </si>
   <si>
-    <t>Introducción a la Programación (Sección asdf)</t>
-  </si>
-  <si>
     <t>Reloj 102</t>
-  </si>
-  <si>
-    <t>Reloj 103</t>
   </si>
   <si>
     <t>Ciencias 507</t>
@@ -549,7 +541,9 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -557,9 +551,11 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -567,10 +563,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -579,42 +575,38 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -637,7 +629,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -674,7 +666,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -685,13 +677,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -699,33 +691,16 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Excel format files
</commit_message>
<xml_diff>
--- a/horario_semestre.xlsx
+++ b/horario_semestre.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Lunes</t>
   </si>
@@ -44,9 +44,23 @@
     <t>10:00</t>
   </si>
   <si>
+    <t>Algoritmos y Complejidad (3)
+Ciencias 506</t>
+  </si>
+  <si>
     <t>11:00</t>
   </si>
   <si>
+    <t>Introducción a la Programación (asdf)
+Reloj 102</t>
+  </si>
+  <si>
+    <t>Algoritmos y Complejidad (3)
+Ciencias 506
+Diseño de Software Verificable (A)
+Humanidades 203</t>
+  </si>
+  <si>
     <t>12:00</t>
   </si>
   <si>
@@ -59,17 +73,9 @@
     <t>14:00</t>
   </si>
   <si>
-    <t>Algoritmos y Complejidad (3)
-Reloj 103</t>
-  </si>
-  <si>
     <t>15:00</t>
   </si>
   <si>
-    <t>Introducción a la Programación (asdf)
-Ciencias 507</t>
-  </si>
-  <si>
     <t>16:00</t>
   </si>
   <si>
@@ -103,13 +109,19 @@
     <t>Introducción a la Programación (Sección asdf)</t>
   </si>
   <si>
+    <t>Diseño de Software Verificable (Sección A)</t>
+  </si>
+  <si>
     <t>Reloj 102</t>
   </si>
   <si>
     <t>Reloj 103</t>
   </si>
   <si>
-    <t>Ciencias 507</t>
+    <t>Ciencias 506</t>
+  </si>
+  <si>
+    <t>Humanidades 203</t>
   </si>
 </sst>
 </file>
@@ -541,36 +553,46 @@
         <v>6</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -579,11 +601,9 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -591,35 +611,27 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -637,7 +649,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -645,24 +657,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -671,15 +683,15 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -688,44 +700,61 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>